<commit_message>
Projektphasen Abschnitt 1: Eingabe und Korrektur
</commit_message>
<xml_diff>
--- a/Documents/Projektphasen.xlsx
+++ b/Documents/Projektphasen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jellef\Documents\GitHub\schoolProject\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30844D2B-7D47-4005-A6CC-BD8DCFE2629A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D2A65F-11EE-4867-B690-4CCD3DDE1154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1035" yWindow="4005" windowWidth="21600" windowHeight="11835" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="45">
   <si>
     <t>Projektphase</t>
   </si>
@@ -165,6 +165,12 @@
   </si>
   <si>
     <t xml:space="preserve">  Speichern in einer Datei.txt</t>
+  </si>
+  <si>
+    <t>Ist</t>
+  </si>
+  <si>
+    <t>Differenz</t>
   </si>
 </sst>
 </file>
@@ -254,13 +260,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -364,11 +371,15 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B0C0BD79-E66C-46D8-A9EA-0C25BAA70075}" name="Tabelle24" displayName="Tabelle24" ref="A2:B39" totalsRowCount="1" headerRowDxfId="1" tableBorderDxfId="0">
-  <autoFilter ref="A2:B38" xr:uid="{0CE74EBA-7DE6-4D07-B11E-D63224CEB0A1}"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B0C0BD79-E66C-46D8-A9EA-0C25BAA70075}" name="Tabelle24" displayName="Tabelle24" ref="A2:D39" totalsRowCount="1" headerRowDxfId="1" tableBorderDxfId="0">
+  <autoFilter ref="A2:D38" xr:uid="{0CE74EBA-7DE6-4D07-B11E-D63224CEB0A1}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{3E2D6C01-6062-4275-943D-E46215700AC6}" name="Projektphase" totalsRowLabel="Gesamtstunden"/>
     <tableColumn id="2" xr3:uid="{E4995326-A6B5-4CE8-A01E-7E78DEA81186}" name="Geplant" totalsRowFunction="sum"/>
+    <tableColumn id="3" xr3:uid="{4327C8FF-12CD-4C6D-BC93-9120CAA0F390}" name="Ist" totalsRowFunction="sum"/>
+    <tableColumn id="4" xr3:uid="{4ABE1F42-6337-48E3-A559-5AD97F414AE5}" name="Differenz" totalsRowFunction="sum">
+      <calculatedColumnFormula>Tabelle24[[#This Row],[Geplant]]-Tabelle24[[#This Row],[Ist]]</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1024,10 +1035,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C3C5FF7-63BF-4F7C-9E67-E750C8103010}">
-  <dimension ref="A2:B39"/>
+  <dimension ref="A2:D39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1035,283 +1046,408 @@
     <col min="1" max="1" width="83.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <f>Tabelle24[[#This Row],[Geplant]]-Tabelle24[[#This Row],[Ist]]</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>34</v>
       </c>
       <c r="B5" s="5">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <f>Tabelle24[[#This Row],[Geplant]]-Tabelle24[[#This Row],[Ist]]</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>35</v>
       </c>
       <c r="B6" s="5">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <f>Tabelle24[[#This Row],[Geplant]]-Tabelle24[[#This Row],[Ist]]</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <f>Tabelle24[[#This Row],[Geplant]]-Tabelle24[[#This Row],[Ist]]</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>0.5</v>
+      </c>
+      <c r="D10">
+        <f>Tabelle24[[#This Row],[Geplant]]-Tabelle24[[#This Row],[Ist]]</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
       <c r="B11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <f>Tabelle24[[#This Row],[Geplant]]-Tabelle24[[#This Row],[Ist]]</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
       <c r="B12">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <f>Tabelle24[[#This Row],[Geplant]]-Tabelle24[[#This Row],[Ist]]</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>42</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <f>Tabelle24[[#This Row],[Geplant]]-Tabelle24[[#This Row],[Ist]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>31</v>
       </c>
       <c r="B15">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <f>Tabelle24[[#This Row],[Geplant]]-Tabelle24[[#This Row],[Ist]]</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>33</v>
       </c>
       <c r="B16">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <f>Tabelle24[[#This Row],[Geplant]]-Tabelle24[[#This Row],[Ist]]</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>32</v>
       </c>
       <c r="B17">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <f>Tabelle24[[#This Row],[Geplant]]-Tabelle24[[#This Row],[Ist]]</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
       <c r="B19">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <f>Tabelle24[[#This Row],[Geplant]]-Tabelle24[[#This Row],[Ist]]</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
       <c r="B20">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <f>Tabelle24[[#This Row],[Geplant]]-Tabelle24[[#This Row],[Ist]]</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>27</v>
       </c>
       <c r="B22">
         <v>15</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <f>Tabelle24[[#This Row],[Geplant]]-Tabelle24[[#This Row],[Ist]]</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>28</v>
       </c>
       <c r="B23">
         <v>30</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <f>Tabelle24[[#This Row],[Geplant]]-Tabelle24[[#This Row],[Ist]]</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>29</v>
       </c>
       <c r="B24">
         <v>30</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <f>Tabelle24[[#This Row],[Geplant]]-Tabelle24[[#This Row],[Ist]]</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>36</v>
       </c>
       <c r="B26">
         <v>15</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <f>Tabelle24[[#This Row],[Geplant]]-Tabelle24[[#This Row],[Ist]]</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>37</v>
       </c>
       <c r="B27">
         <v>5</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <f>Tabelle24[[#This Row],[Geplant]]-Tabelle24[[#This Row],[Ist]]</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>38</v>
       </c>
       <c r="B28">
         <v>8.5</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <f>Tabelle24[[#This Row],[Geplant]]-Tabelle24[[#This Row],[Ist]]</f>
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>13</v>
       </c>
       <c r="B29">
         <v>20</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <f>Tabelle24[[#This Row],[Geplant]]-Tabelle24[[#This Row],[Ist]]</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>14</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D31">
+        <f>Tabelle24[[#This Row],[Geplant]]-Tabelle24[[#This Row],[Ist]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>15</v>
       </c>
       <c r="B32">
         <v>4</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <f>Tabelle24[[#This Row],[Geplant]]-Tabelle24[[#This Row],[Ist]]</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>16</v>
       </c>
       <c r="B33">
         <v>9</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <f>Tabelle24[[#This Row],[Geplant]]-Tabelle24[[#This Row],[Ist]]</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>17</v>
       </c>
       <c r="B34">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <f>Tabelle24[[#This Row],[Geplant]]-Tabelle24[[#This Row],[Ist]]</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>19</v>
       </c>
       <c r="B36">
         <v>4</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <f>Tabelle24[[#This Row],[Geplant]]-Tabelle24[[#This Row],[Ist]]</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>20</v>
       </c>
       <c r="B37">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <f>Tabelle24[[#This Row],[Geplant]]-Tabelle24[[#This Row],[Ist]]</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>18</v>
       </c>
       <c r="B38">
         <v>10</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D38">
+        <f>Tabelle24[[#This Row],[Geplant]]-Tabelle24[[#This Row],[Ist]]</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>9</v>
       </c>
       <c r="B39">
         <f>SUBTOTAL(109,Tabelle24[Geplant])</f>
         <v>224</v>
+      </c>
+      <c r="C39">
+        <f>SUBTOTAL(109,Tabelle24[Ist])</f>
+        <v>0.5</v>
+      </c>
+      <c r="D39">
+        <f>SUBTOTAL(109,Tabelle24[Differenz])</f>
+        <v>223.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>